<commit_message>
Changing data from BioPortal to DOH.
</commit_message>
<xml_diff>
--- a/data/pop_estUS.xlsx
+++ b/data/pop_estUS.xlsx
@@ -1,65 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marytorres/Documents/covid19-vuln/data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0127D6D7-CA90-2C4B-96F1-03943C390504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="460" windowWidth="10400" windowHeight="9860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>ageRange</t>
+    <t xml:space="preserve">AGE</t>
   </si>
   <si>
-    <t>30 to 39</t>
-  </si>
-  <si>
-    <t>40 to 49</t>
-  </si>
-  <si>
-    <t>50 to 64</t>
-  </si>
-  <si>
-    <t>65 to 74</t>
-  </si>
-  <si>
-    <t>pop_est</t>
-  </si>
-  <si>
-    <t>0 to 29</t>
+    <t xml:space="preserve">hispanics</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -95,15 +61,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -385,65 +342,671 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="158" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
-    </sheetView>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>970381</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>985785</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>996643</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1012068</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1034924</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="B7" t="n">
+        <v>1035977</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
         <v>6</v>
       </c>
-      <c r="B2">
-        <v>30516828</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>9178580</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>8091692</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>8643959</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>2978586</v>
+      <c r="B8" t="n">
+        <v>1026037</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1022614</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1031178</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1056664</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1063799</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1055870</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1089410</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1090489</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>1069134</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>1048645</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>1028660</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>1013557</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>1003432</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>1012132</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>1014155</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>984889</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>973536</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>968018</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="n">
+        <v>966689</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="n">
+        <v>978137</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
+        <v>987882</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>991990</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>1006847</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n">
+        <v>997286</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="n">
+        <v>982945</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="n">
+        <v>932568</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="n">
+        <v>924234</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="n">
+        <v>910239</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="n">
+        <v>915195</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="n">
+        <v>919407</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="n">
+        <v>891673</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="n">
+        <v>905417</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="n">
+        <v>905823</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="n">
+        <v>891079</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="n">
+        <v>914266</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="n">
+        <v>842041</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="n">
+        <v>836122</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="n">
+        <v>826755</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="n">
+        <v>810307</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="n">
+        <v>814626</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="n">
+        <v>777769</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="n">
+        <v>764924</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="n">
+        <v>755613</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="n">
+        <v>749269</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="n">
+        <v>743974</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="n">
+        <v>691127</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="n">
+        <v>672048</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="n">
+        <v>644630</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="n">
+        <v>636252</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="n">
+        <v>639948</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="n">
+        <v>612519</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="n">
+        <v>582377</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="n">
+        <v>557871</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="n">
+        <v>533950</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="n">
+        <v>533033</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="n">
+        <v>484129</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="n">
+        <v>456045</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="n">
+        <v>438853</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="n">
+        <v>417203</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="n">
+        <v>402524</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="n">
+        <v>366344</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="n">
+        <v>340175</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="n">
+        <v>314190</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="n">
+        <v>301834</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" t="n">
+        <v>290151</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" t="n">
+        <v>265238</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" t="n">
+        <v>252893</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" t="n">
+        <v>239034</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>74</v>
+      </c>
+      <c r="B76" t="n">
+        <v>206203</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>75</v>
+      </c>
+      <c r="B77" t="n">
+        <v>193774</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>76</v>
+      </c>
+      <c r="B78" t="n">
+        <v>175934</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>77</v>
+      </c>
+      <c r="B79" t="n">
+        <v>165862</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>78</v>
+      </c>
+      <c r="B80" t="n">
+        <v>147751</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>79</v>
+      </c>
+      <c r="B81" t="n">
+        <v>136832</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>80</v>
+      </c>
+      <c r="B82" t="n">
+        <v>130175</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>